<commit_message>
add overtime salary coff
</commit_message>
<xml_diff>
--- a/时薪计算器.xlsx
+++ b/时薪计算器.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\03_personal\05_work\hourly-salary-calculator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51D3BB00-200D-450E-9D4D-2FDD62BA0049}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90022B90-1E0E-483B-8F98-AE0DC83EF3C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1800" yWindow="5715" windowWidth="28800" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2250" yWindow="4545" windowWidth="28800" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>个人</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -123,10 +123,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>从出门到归家门的小时数</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>每月工作日数</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -179,6 +175,26 @@
   </si>
   <si>
     <t>欢迎到github页面提供意见，如有帮助，欢迎点赞⭐</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>每日通勤时间（往返）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>加班工资系数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>超过10的部分算加班</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>每日工作时间（上班到下班）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -255,22 +271,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -553,322 +582,405 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L30"/>
+  <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.625" customWidth="1"/>
+    <col min="1" max="1" width="25.375" customWidth="1"/>
     <col min="2" max="2" width="10.375" customWidth="1"/>
-    <col min="3" max="3" width="11.125" customWidth="1"/>
-    <col min="4" max="4" width="21" customWidth="1"/>
-    <col min="5" max="5" width="31.5" customWidth="1"/>
+    <col min="3" max="3" width="13.25" customWidth="1"/>
+    <col min="4" max="4" width="18.375" customWidth="1"/>
+    <col min="5" max="5" width="39.625" customWidth="1"/>
     <col min="10" max="10" width="14.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="5" t="s">
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="7">
+        <v>0.02</v>
+      </c>
+      <c r="C3" s="7">
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="D3" s="8">
+        <v>0.02</v>
+      </c>
+      <c r="E3" s="5"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="7">
+        <v>0.08</v>
+      </c>
+      <c r="C4" s="7">
+        <v>0.16</v>
+      </c>
+      <c r="D4" s="8">
+        <v>0</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="7">
+        <v>0</v>
+      </c>
+      <c r="C5" s="7">
+        <v>9.5999999999999992E-3</v>
+      </c>
+      <c r="D5" s="8">
+        <v>0</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="7">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="C6" s="7">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="D6" s="8">
+        <v>0</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="7">
+        <v>0</v>
+      </c>
+      <c r="C7" s="7">
+        <v>0</v>
+      </c>
+      <c r="D7" s="8">
+        <v>0</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="8">
+        <f>B15</f>
+        <v>0.05</v>
+      </c>
+      <c r="C8" s="8">
+        <f>B15</f>
+        <v>0.05</v>
+      </c>
+      <c r="D8" s="8">
+        <f>B8+C8</f>
+        <v>0.1</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9" s="5"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="5"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="9">
+        <v>22000</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="5">
+        <v>2</v>
+      </c>
+      <c r="E12" s="5"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="9">
+        <v>3604</v>
+      </c>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="9">
+        <v>1700</v>
+      </c>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="9">
+        <v>0</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2">
-        <v>0.02</v>
-      </c>
-      <c r="C3" s="2">
-        <v>8.6999999999999994E-2</v>
-      </c>
-      <c r="D3" s="1">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="2">
-        <v>0.08</v>
-      </c>
-      <c r="C4" s="2">
-        <v>0.16</v>
-      </c>
-      <c r="D4" s="1">
-        <v>0</v>
-      </c>
-      <c r="E4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="2">
-        <v>0</v>
-      </c>
-      <c r="C5" s="2">
-        <v>9.5999999999999992E-3</v>
-      </c>
-      <c r="D5" s="1">
-        <v>0</v>
-      </c>
-      <c r="E5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="2">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="C6" s="2">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="D6" s="1">
-        <v>0</v>
-      </c>
-      <c r="E6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="2">
-        <v>0</v>
-      </c>
-      <c r="C7" s="2">
-        <v>0</v>
-      </c>
-      <c r="D7" s="1">
-        <v>0</v>
-      </c>
-      <c r="E7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1">
-        <f>B15</f>
-        <v>0.12</v>
-      </c>
-      <c r="C8" s="1">
-        <f>B15</f>
-        <v>0.12</v>
-      </c>
-      <c r="D8" s="1">
-        <f>B8+C8</f>
-        <v>0.24</v>
-      </c>
-      <c r="E8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="3">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="3">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="3">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="2">
-        <v>0.12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>20</v>
-      </c>
-      <c r="B16" s="3">
-        <v>300</v>
-      </c>
-      <c r="C16" s="7" t="s">
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="9">
+        <v>22000</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17" s="3">
-        <v>20000</v>
-      </c>
-      <c r="C17" s="7" t="s">
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="9">
+        <v>1.5</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="9">
+        <v>10</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="3">
-        <v>11</v>
-      </c>
-      <c r="C18" s="7" t="s">
+      <c r="B20" s="9">
+        <v>21.75</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="5"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>23</v>
-      </c>
-      <c r="B19" s="3">
-        <v>21.75</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="B23" s="10">
+        <f>(12*(B12-(SUM(B3:B7)-SUM(D3:D7))*B13+B14*B15+B16)+B17)/(12*(B18+MAX(0,(B19-10))*D12+MIN(B19,10))*(MAX(0,(B20-21.75))*D12+MIN(21.75,B20)))</f>
+        <v>94.429590538064289</v>
+      </c>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" s="10">
+        <f>B12-(SUM(B3:B7)-SUM(D3:D7))*B13+B14*B15+B16</f>
+        <v>21785.867999999999</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25" s="10">
+        <f>(12*(B12-(SUM(B3:B7)-SUM(D3:D7))*B13+B14*B15+B16)+B17)</f>
+        <v>283430.41599999997</v>
+      </c>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="10">
+        <f>B12+SUM(C3:C7)*B13+B14*B15+B16</f>
+        <v>23035.0144</v>
+      </c>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>32</v>
-      </c>
-      <c r="B22" s="4">
-        <f>(12*(B12-(SUM(B3:B7)-SUM(D3:D7))*B13+B14*B15+B16)+B17)/(12*B18*B19)</f>
-        <v>51.563915012190876</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>33</v>
-      </c>
-      <c r="B23" s="4">
-        <f>B12-(SUM(B3:B7)-SUM(D3:D7))*B13+B14*B15+B16</f>
-        <v>10670</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+      <c r="B27" s="10">
+        <f>12*B26+B17</f>
+        <v>298420.1728</v>
+      </c>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="2"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B24" s="4">
-        <f>(12*(B12-(SUM(B3:B7)-SUM(D3:D7))*B13+B14*B15+B16)+B17)</f>
-        <v>148040</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>27</v>
-      </c>
-      <c r="B25" s="4">
-        <f>B12+SUM(C3:C7)*B13+B14*B15+B16</f>
-        <v>14136</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>26</v>
-      </c>
-      <c r="B26" s="4">
-        <f>12*B25+B17</f>
-        <v>189632</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B29" s="9"/>
-      <c r="C29" s="9"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="8"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A29:D29"/>
+  <mergeCells count="7">
+    <mergeCell ref="A30:D30"/>
     <mergeCell ref="A1:D1"/>
-    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="C20:E20"/>
     <mergeCell ref="C18:E18"/>
     <mergeCell ref="C16:E16"/>
     <mergeCell ref="C17:E17"/>
+    <mergeCell ref="C19:E19"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="A30:E30" r:id="rId1" display="https://github.com/Ancho5515/hourly-salary-calculator" xr:uid="{0A914194-44EE-498C-9503-C9086346C427}"/>
+    <hyperlink ref="A31:E31" r:id="rId1" display="https://github.com/Ancho5515/hourly-salary-calculator" xr:uid="{0A914194-44EE-498C-9503-C9086346C427}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>

</xml_diff>